<commit_message>
Updated file structure and paths
</commit_message>
<xml_diff>
--- a/Datafiles/Simulation Passive and Active properties.xlsx
+++ b/Datafiles/Simulation Passive and Active properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\OneDrive - Drexel University\Documents\Kenyon_cell_work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\OneDrive - Drexel University\Documents\KC_NaChBac_Model\Datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E684A103-509F-4956-91BE-B92BCA4C0ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4770132-F594-4724-871D-F9808CBF5B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>WT</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>nachbac_everywhere</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
 </sst>
 </file>
@@ -439,7 +436,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,8 +655,8 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
+      <c r="B5">
+        <v>14</v>
       </c>
       <c r="C5">
         <v>125</v>

</xml_diff>